<commit_message>
Quality control completed for CPI_Colitis samples
</commit_message>
<xml_diff>
--- a/Data Overview.xlsx
+++ b/Data Overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Esmaeil\scRNA-seq\Single-Cell-Pipeline-in-R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25939A46-4B89-4A16-A459-36EF140C9401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417228FC-6AC8-4D06-ACCC-70DF232131BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B9214421-C7AA-466F-926C-CBCB7BD6B19D}"/>
+    <workbookView xWindow="-27330" yWindow="2520" windowWidth="24780" windowHeight="11295" activeTab="2" xr2:uid="{B9214421-C7AA-466F-926C-CBCB7BD6B19D}"/>
   </bookViews>
   <sheets>
     <sheet name="Part 1 (22 Samples)" sheetId="1" r:id="rId1"/>
@@ -404,12 +404,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -424,8 +442,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1004,7 +1025,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1017,10 +1038,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C1" t="s">
@@ -1034,7 +1055,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B2" t="s">
@@ -1051,7 +1072,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B3" t="s">
@@ -1068,7 +1089,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B4" t="s">
@@ -1085,7 +1106,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B5" t="s">
@@ -1102,7 +1123,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B6" t="s">
@@ -1119,7 +1140,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B7" t="s">
@@ -1136,7 +1157,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B8" t="s">
@@ -1153,7 +1174,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B9" t="s">
@@ -1167,7 +1188,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>56</v>
       </c>
       <c r="B10" t="s">
@@ -1178,7 +1199,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B11" t="s">
@@ -1189,7 +1210,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B12" t="s">
@@ -1200,7 +1221,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B13" t="s">
@@ -1211,7 +1232,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B14" t="s">
@@ -1222,7 +1243,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B15" t="s">
@@ -1230,7 +1251,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B16" t="s">
@@ -1238,27 +1259,27 @@
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Quality control completed for UC Inflamed samples
</commit_message>
<xml_diff>
--- a/Data Overview.xlsx
+++ b/Data Overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Esmaeil\scRNA-seq\Single-Cell-Pipeline-in-R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B54A3F-1005-42E8-91E7-D4E5B2CAB22A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB2B0ED-8B37-4ADF-8484-7A35BBD98223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27330" yWindow="2520" windowWidth="24780" windowHeight="11295" activeTab="2" xr2:uid="{B9214421-C7AA-466F-926C-CBCB7BD6B19D}"/>
+    <workbookView xWindow="-26625" yWindow="2460" windowWidth="24780" windowHeight="11295" activeTab="2" xr2:uid="{B9214421-C7AA-466F-926C-CBCB7BD6B19D}"/>
   </bookViews>
   <sheets>
     <sheet name="Part 1 (22 Samples)" sheetId="1" r:id="rId1"/>
@@ -1025,7 +1025,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1047,7 +1047,7 @@
       <c r="C1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>93</v>
       </c>
       <c r="E1" t="s">
@@ -1064,7 +1064,7 @@
       <c r="C2" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>94</v>
       </c>
       <c r="E2" t="s">
@@ -1081,7 +1081,7 @@
       <c r="C3" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>95</v>
       </c>
       <c r="E3" t="s">
@@ -1098,7 +1098,7 @@
       <c r="C4" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>96</v>
       </c>
       <c r="E4" t="s">
@@ -1115,7 +1115,7 @@
       <c r="C5" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>97</v>
       </c>
       <c r="E5" t="s">
@@ -1129,10 +1129,10 @@
       <c r="B6" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>98</v>
       </c>
       <c r="E6" t="s">
@@ -1146,10 +1146,10 @@
       <c r="B7" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>99</v>
       </c>
       <c r="E7" t="s">
@@ -1163,7 +1163,7 @@
       <c r="B8" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>85</v>
       </c>
       <c r="D8" t="s">
@@ -1180,7 +1180,7 @@
       <c r="B9" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="3" t="s">
         <v>84</v>
       </c>
       <c r="D9" t="s">

</xml_diff>

<commit_message>
Quality control completed for UC Non Inflamed samples
</commit_message>
<xml_diff>
--- a/Data Overview.xlsx
+++ b/Data Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Esmaeil\scRNA-seq\Single-Cell-Pipeline-in-R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB2B0ED-8B37-4ADF-8484-7A35BBD98223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97629656-ED07-428A-8845-84275BED7034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-26625" yWindow="2460" windowWidth="24780" windowHeight="11295" activeTab="2" xr2:uid="{B9214421-C7AA-466F-926C-CBCB7BD6B19D}"/>
   </bookViews>
@@ -1025,7 +1025,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1050,7 +1050,7 @@
       <c r="D1" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>114</v>
       </c>
     </row>
@@ -1067,7 +1067,7 @@
       <c r="D2" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>113</v>
       </c>
     </row>
@@ -1084,7 +1084,7 @@
       <c r="D3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       <c r="D4" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1118,7 +1118,7 @@
       <c r="D5" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1135,7 +1135,7 @@
       <c r="D6" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1152,7 +1152,7 @@
       <c r="D7" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1166,10 +1166,10 @@
       <c r="C8" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1183,7 +1183,7 @@
       <c r="C9" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>101</v>
       </c>
     </row>
@@ -1194,7 +1194,7 @@
       <c r="B10" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>102</v>
       </c>
     </row>
@@ -1205,7 +1205,7 @@
       <c r="B11" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1216,7 +1216,7 @@
       <c r="B12" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>104</v>
       </c>
     </row>
@@ -1227,7 +1227,7 @@
       <c r="B13" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="3" t="s">
         <v>105</v>
       </c>
     </row>
@@ -1238,7 +1238,7 @@
       <c r="B14" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
         <v>106</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Merged all individual samples into a single Seurat object and performed basic analysis (normalization, variable feature selection, scaling, PCA). Ready for downstream integration.
</commit_message>
<xml_diff>
--- a/Data Overview.xlsx
+++ b/Data Overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Esmaeil\scRNA-seq\Single-Cell-Pipeline-in-R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97629656-ED07-428A-8845-84275BED7034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3059445B-2F5D-42B2-ACB5-75129C347F34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-26625" yWindow="2460" windowWidth="24780" windowHeight="11295" activeTab="2" xr2:uid="{B9214421-C7AA-466F-926C-CBCB7BD6B19D}"/>
   </bookViews>
@@ -1025,7 +1025,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Plotted UMAP after dataset integration and clustering
</commit_message>
<xml_diff>
--- a/Data Overview.xlsx
+++ b/Data Overview.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Esmaeil\scRNA-seq\Single-Cell-Pipeline-in-R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Esmaeil\irAEsProject\irAEsProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A662018C-69D5-46C6-8074-451BDC3AAAEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479E040E-725E-4432-A421-3FAD8C6173B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B9214421-C7AA-466F-926C-CBCB7BD6B19D}"/>
+    <workbookView xWindow="-25935" yWindow="1965" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{B9214421-C7AA-466F-926C-CBCB7BD6B19D}"/>
   </bookViews>
   <sheets>
     <sheet name="Part 1 (22 Samples)" sheetId="1" r:id="rId1"/>
@@ -784,7 +784,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC9C76D-68B1-4601-AF75-A15430F3E4F1}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,9 +1024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3038858-7A36-44C0-BC21-C5215BBD1362}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Find Markers with Wilcoxon test completed
</commit_message>
<xml_diff>
--- a/Data Overview.xlsx
+++ b/Data Overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Esmaeil\irAEsProject\irAEsProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{479E040E-725E-4432-A421-3FAD8C6173B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6F1927-44DE-4DDE-AF8A-5B8C2B14D9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25935" yWindow="1965" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{B9214421-C7AA-466F-926C-CBCB7BD6B19D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B9214421-C7AA-466F-926C-CBCB7BD6B19D}"/>
   </bookViews>
   <sheets>
     <sheet name="Part 1 (22 Samples)" sheetId="1" r:id="rId1"/>
@@ -886,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC9C76D-68B1-4601-AF75-A15430F3E4F1}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="A1:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,7 +1024,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3038858-7A36-44C0-BC21-C5215BBD1362}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
load and combine TCR data for Dataset 1 (Adrienne) with scRepertoire
</commit_message>
<xml_diff>
--- a/Data Overview.xlsx
+++ b/Data Overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Esmaeil\irAEsProject\irAEsProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B5D2E4-54F2-4D35-9A32-81C422FED8D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FAC5C31-E703-4773-9F2D-3FDA0233E4C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{B9214421-C7AA-466F-926C-CBCB7BD6B19D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B9214421-C7AA-466F-926C-CBCB7BD6B19D}"/>
   </bookViews>
   <sheets>
     <sheet name="Part 1 (22 Samples)" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
   <si>
     <t>"+CPI no colitis NC1"</t>
   </si>
@@ -418,6 +418,21 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>"+CPI no colitis NC2"</t>
+  </si>
+  <si>
+    <t>"+CPI no colitis NC3"</t>
+  </si>
+  <si>
+    <t>"+CPI no colitis NC4"</t>
+  </si>
+  <si>
+    <t>"+CPI no colitis NC5"</t>
+  </si>
+  <si>
+    <t>"+CPI no colitis NC6"</t>
   </si>
 </sst>
 </file>
@@ -818,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0AE116-18EB-4A08-857A-49F55D141671}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,7 +872,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -868,7 +883,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>127</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -879,7 +894,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -890,7 +905,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>0</v>
+        <v>129</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
@@ -901,7 +916,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="C7" t="s">
         <v>125</v>
@@ -1379,7 +1394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DCD8D23-D9ED-419F-8C24-03AD498F59F4}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Update loading TCR data for Dataset 1 (Adrienne) with scRepertoire
</commit_message>
<xml_diff>
--- a/Data Overview.xlsx
+++ b/Data Overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Esmaeil\irAEsProject\irAEsProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FAC5C31-E703-4773-9F2D-3FDA0233E4C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7A287E-8B52-4309-A828-E4B6BAB4189F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B9214421-C7AA-466F-926C-CBCB7BD6B19D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B9214421-C7AA-466F-926C-CBCB7BD6B19D}"/>
   </bookViews>
   <sheets>
     <sheet name="Part 1 (22 Samples)" sheetId="1" r:id="rId1"/>
@@ -833,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0AE116-18EB-4A08-857A-49F55D141671}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,8 +1096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3038858-7A36-44C0-BC21-C5215BBD1362}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Start QC and integration Dataset 4
</commit_message>
<xml_diff>
--- a/Data Overview.xlsx
+++ b/Data Overview.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Esmaeil\irAEsProject\irAEsProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19687476-5574-4CAA-B23D-51C35E99E525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FA7259-3DE8-4312-BFFD-7E5BC81A6934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B9214421-C7AA-466F-926C-CBCB7BD6B19D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B9214421-C7AA-466F-926C-CBCB7BD6B19D}"/>
   </bookViews>
   <sheets>
     <sheet name="Part 1 (22 Samples)" sheetId="1" r:id="rId1"/>
     <sheet name="Part 2 (30 Samples)" sheetId="2" r:id="rId2"/>
     <sheet name="Part 3 (68 Samples)" sheetId="3" r:id="rId3"/>
-    <sheet name="Part 4" sheetId="4" r:id="rId4"/>
-    <sheet name="Part 5" sheetId="5" r:id="rId5"/>
+    <sheet name="Part 4 (14 Samples)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="138">
   <si>
     <t>"+CPI no colitis NC1"</t>
   </si>
@@ -384,30 +383,6 @@
     <t>"UC Non Inflamed 1_New"</t>
   </si>
   <si>
-    <t>Healthy individuals without immunotherapy treatment and no colitis (baseline control group).</t>
-  </si>
-  <si>
-    <t>Patients receiving Immune Checkpoint Inhibitors (CPI) treatment but without colitis.</t>
-  </si>
-  <si>
-    <t>Patients treated with CPI who developed colitis as an immune-related adverse event.</t>
-  </si>
-  <si>
-    <t>Healthy controls without any treatment and no colitis.</t>
-  </si>
-  <si>
-    <t>Patients undergoing Immune Checkpoint Inhibitor (ICI) therapy without colitis.</t>
-  </si>
-  <si>
-    <t>Patients on ICI therapy who developed immune-related colitis.</t>
-  </si>
-  <si>
-    <t>Patients treated with CPI who experienced irAE-associated colitis.</t>
-  </si>
-  <si>
-    <t>Patients receiving CPI treatment but without colitis.</t>
-  </si>
-  <si>
     <t>Healthy individuals with no treatment and no colitis.</t>
   </si>
   <si>
@@ -417,9 +392,6 @@
     <t>Patients with Ulcerative Colitis in remission or non-inflamed phase.</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>"+CPI no colitis NC2"</t>
   </si>
   <si>
@@ -433,13 +405,61 @@
   </si>
   <si>
     <t>"+CPI no colitis NC6"</t>
+  </si>
+  <si>
+    <t>"Jun_srobj_2"</t>
+  </si>
+  <si>
+    <t>"Jun_srobj_1"</t>
+  </si>
+  <si>
+    <t>"Jun_srobj_4"</t>
+  </si>
+  <si>
+    <t>"Jun_srobj_5"</t>
+  </si>
+  <si>
+    <t>"Jun_srobj_7"</t>
+  </si>
+  <si>
+    <t>"Jun_srobj_8"</t>
+  </si>
+  <si>
+    <t>"Jun_srobj_9"</t>
+  </si>
+  <si>
+    <t>"Jun_srobj_3"</t>
+  </si>
+  <si>
+    <t>"Jun_srobj_10"</t>
+  </si>
+  <si>
+    <t>"Jun_srobj_11"</t>
+  </si>
+  <si>
+    <t>"Jun_srobj_12"</t>
+  </si>
+  <si>
+    <t>"Jun_srobj_13"</t>
+  </si>
+  <si>
+    <t>"Jun_srobj_14"</t>
+  </si>
+  <si>
+    <t>"Jun_srobj_15"</t>
+  </si>
+  <si>
+    <t>Patients receiving Immune Checkpoint Inhibitors therapy  without colitis.</t>
+  </si>
+  <si>
+    <t>Patients receiving Immune Checkpoint Inhibitors therapy who developed colitis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,6 +469,19 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -492,11 +525,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -833,14 +868,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A0AE116-18EB-4A08-857A-49F55D141671}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="83" customWidth="1"/>
-    <col min="2" max="2" width="74.7109375" customWidth="1"/>
+    <col min="1" max="1" width="46.7109375" customWidth="1"/>
+    <col min="2" max="2" width="64.28515625" customWidth="1"/>
     <col min="3" max="3" width="74.85546875" customWidth="1"/>
     <col min="4" max="4" width="23.140625" customWidth="1"/>
   </cols>
@@ -850,10 +885,10 @@
         <v>114</v>
       </c>
       <c r="B1" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
       <c r="C1" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -872,7 +907,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -883,7 +918,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -894,7 +929,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -905,7 +940,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
@@ -916,10 +951,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C7" t="s">
-        <v>125</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -927,15 +962,12 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -953,20 +985,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.7109375" customWidth="1"/>
-    <col min="2" max="2" width="70.85546875" customWidth="1"/>
-    <col min="3" max="3" width="56.140625" customWidth="1"/>
+    <col min="1" max="1" width="46.85546875" customWidth="1"/>
+    <col min="2" max="2" width="64.140625" customWidth="1"/>
+    <col min="3" max="3" width="87" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C1" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1096,45 +1128,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3038858-7A36-44C0-BC21-C5215BBD1362}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="60.7109375" customWidth="1"/>
-    <col min="2" max="2" width="44.7109375" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" customWidth="1"/>
-    <col min="4" max="4" width="55.85546875" customWidth="1"/>
-    <col min="5" max="5" width="59.5703125" customWidth="1"/>
+    <col min="1" max="1" width="46.7109375" customWidth="1"/>
+    <col min="2" max="2" width="64.42578125" customWidth="1"/>
+    <col min="3" max="3" width="70.7109375" customWidth="1"/>
+    <col min="4" max="4" width="57" customWidth="1"/>
+    <col min="5" max="5" width="62" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="C1" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="D1" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E1" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>46</v>
+        <v>91</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>67</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>92</v>
@@ -1145,13 +1177,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>68</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>90</v>
+        <v>47</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>93</v>
@@ -1161,14 +1193,14 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>48</v>
+      <c r="A4" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>89</v>
+      <c r="C4" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>94</v>
@@ -1178,14 +1210,14 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>49</v>
+      <c r="A5" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>88</v>
+      <c r="C5" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>95</v>
@@ -1195,14 +1227,14 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>50</v>
+      <c r="A6" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>87</v>
+      <c r="C6" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>96</v>
@@ -1212,14 +1244,14 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>51</v>
+      <c r="A7" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>86</v>
+      <c r="C7" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>97</v>
@@ -1230,13 +1262,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>73</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>98</v>
@@ -1246,14 +1278,14 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>53</v>
+      <c r="A9" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>84</v>
+      <c r="C9" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>99</v>
@@ -1263,112 +1295,112 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>54</v>
+      <c r="A10" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>83</v>
+      <c r="C10" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="B11" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="C11" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="D11" s="1" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="B12" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="C12" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="D12" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="B13" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="D13" s="3" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="B14" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="D14" s="3" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="B15" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="D15" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="B16" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>61</v>
-      </c>
+      <c r="C16" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="C17" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1380,24 +1412,105 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6F10C5-3932-4272-A80F-198CD87810B3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DCD8D23-D9ED-419F-8C24-03AD498F59F4}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="48.7109375" customWidth="1"/>
+    <col min="2" max="2" width="81.85546875" customWidth="1"/>
+    <col min="3" max="3" width="67.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="5"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
QC Done | All datasets
</commit_message>
<xml_diff>
--- a/Data Overview.xlsx
+++ b/Data Overview.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Esmaeil\irAEsProject\irAEsProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FA7259-3DE8-4312-BFFD-7E5BC81A6934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BDF909-72A5-44C8-B4AB-F46D9819ABBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B9214421-C7AA-466F-926C-CBCB7BD6B19D}"/>
   </bookViews>
   <sheets>
     <sheet name="Part 1 (22 Samples)" sheetId="1" r:id="rId1"/>
     <sheet name="Part 2 (30 Samples)" sheetId="2" r:id="rId2"/>
-    <sheet name="Part 3 (68 Samples)" sheetId="3" r:id="rId3"/>
+    <sheet name="Part 3 (26 Samples)" sheetId="3" r:id="rId3"/>
     <sheet name="Part 4 (14 Samples)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -1129,7 +1129,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>